<commit_message>
Use Case Diagram and Req Fixes
Created Use Case Diagram exported as png and drawio file for any future edits

Fixed Typos and made some descriptions clearer in Requirements
</commit_message>
<xml_diff>
--- a/EMS Requirements.xlsx
+++ b/EMS Requirements.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25825"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D39EF27C-EEFD-42F5-8D13-615ADF7FAB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\EmployeeManagementSystem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568D1B73-1447-4395-A779-4EADEA86DF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -61,9 +64,6 @@
     <t>Oct. 30</t>
   </si>
   <si>
-    <t>Manager can register an employee to a position, adding them to the system</t>
-  </si>
-  <si>
     <t>Essential</t>
   </si>
   <si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Manager can remove an employee from their team</t>
-  </si>
-  <si>
-    <t>Manager can remove an employee from the system</t>
   </si>
   <si>
     <t>Employee</t>
@@ -131,15 +128,6 @@
     <t>Important</t>
   </si>
   <si>
-    <t>Manager can override employee hours for past and future (misreport, sick, coming vacation, etc)</t>
-  </si>
-  <si>
-    <t>2.2 2.4</t>
-  </si>
-  <si>
-    <t>System notifies if Manager is overriding existing value and checks to ensure override is confimred</t>
-  </si>
-  <si>
     <t>3.3</t>
   </si>
   <si>
@@ -147,13 +135,29 @@
   </si>
   <si>
     <t>Project Details can be summarized such as start and end date, hrs worked, etc</t>
+  </si>
+  <si>
+    <t>Admin can register an employee adding them to the system</t>
+  </si>
+  <si>
+    <t>Admin can remove/make inactive an employee from the system</t>
+  </si>
+  <si>
+    <t>Manager can override/correct employee hours for past and future (misreport, sick, coming vacation, etc)</t>
+  </si>
+  <si>
+    <t>System notifies if Manager is overriding existing value and checks to ensure override is confirmed</t>
+  </si>
+  <si>
+    <t>2.2
+2.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,10 +530,10 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
@@ -540,7 +544,7 @@
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -566,67 +570,67 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30.75">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30.75">
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30.75">
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -636,17 +640,17 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.5</v>
       </c>
@@ -656,111 +660,111 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.6</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.1</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2.2000000000000002</v>
       </c>
       <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30.75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2.2999999999999998</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30.75">
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2.4</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30.75">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3.1</v>
       </c>
@@ -771,13 +775,13 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3.2</v>
       </c>
@@ -788,13 +792,13 @@
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30.75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3.3</v>
       </c>
@@ -802,19 +806,20 @@
         <v>8</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30.75">
+        <v>30</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3.4</v>
       </c>
@@ -822,19 +827,19 @@
         <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4.0999999999999996</v>
       </c>
@@ -842,16 +847,16 @@
         <v>8</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4.2</v>
       </c>
@@ -859,19 +864,20 @@
         <v>8</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>